<commit_message>
updated with latest model
</commit_message>
<xml_diff>
--- a/data/labelling-catalog.xlsx
+++ b/data/labelling-catalog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rakesh_poduval/repositories/prodatalytics-repos/automated-inventory-monitoring/development/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rakesh_poduval/repositories/prodatalytics-repos/automated-inventory-monitoring/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D89AD8-0274-E24C-9990-B8FB1732A4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{085D6BD8-4DA6-324E-8DFE-044A180B35C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="-3040" windowWidth="38400" windowHeight="21100" xr2:uid="{FBF291A4-CA4D-794B-B3BB-BDD97ADC7B2C}"/>
+    <workbookView xWindow="-38400" yWindow="1660" windowWidth="38400" windowHeight="18760" xr2:uid="{FBF291A4-CA4D-794B-B3BB-BDD97ADC7B2C}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>brand</t>
   </si>
@@ -55,117 +55,21 @@
     <t>category</t>
   </si>
   <si>
-    <t>personal care</t>
-  </si>
-  <si>
-    <t>hair care</t>
-  </si>
-  <si>
-    <t>head &amp; shoulders</t>
-  </si>
-  <si>
     <t>oral care</t>
   </si>
   <si>
-    <t>beverages</t>
-  </si>
-  <si>
     <t>dairy drinks</t>
   </si>
   <si>
-    <t>epigamia</t>
-  </si>
-  <si>
     <t>hair oil</t>
   </si>
   <si>
-    <t>parachute</t>
-  </si>
-  <si>
-    <t>grocery</t>
-  </si>
-  <si>
     <t>staples</t>
   </si>
   <si>
-    <t>unbranded</t>
-  </si>
-  <si>
-    <t>snacks</t>
-  </si>
-  <si>
-    <t>chips</t>
-  </si>
-  <si>
-    <t>lays</t>
-  </si>
-  <si>
-    <t>fruit drinks</t>
-  </si>
-  <si>
-    <t>maaza</t>
-  </si>
-  <si>
-    <t>packaged water</t>
-  </si>
-  <si>
-    <t>aquafina</t>
-  </si>
-  <si>
-    <t>20% discount pack</t>
-  </si>
-  <si>
-    <t>80 ml</t>
-  </si>
-  <si>
-    <t>1 piece</t>
-  </si>
-  <si>
-    <t>300 ml</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>40 gm</t>
-  </si>
-  <si>
-    <t>1.2 L</t>
-  </si>
-  <si>
-    <t>20 Rs.</t>
-  </si>
-  <si>
-    <t>1 L</t>
-  </si>
-  <si>
-    <t>sku_1</t>
-  </si>
-  <si>
-    <t>sku_2</t>
-  </si>
-  <si>
-    <t>sku_3</t>
-  </si>
-  <si>
-    <t>sku_4</t>
-  </si>
-  <si>
-    <t>sku_5</t>
-  </si>
-  <si>
-    <t>sku_6</t>
-  </si>
-  <si>
-    <t>sku_7</t>
-  </si>
-  <si>
-    <t>sku_8</t>
-  </si>
-  <si>
-    <t>sku_9</t>
-  </si>
-  <si>
     <t>price_per_unit</t>
   </si>
   <si>
@@ -175,59 +79,80 @@
     <t>additional_info</t>
   </si>
   <si>
-    <t>hs_shampoo_bottle</t>
-  </si>
-  <si>
-    <t>oral_b</t>
-  </si>
-  <si>
-    <t>epigamia_milkshake_strawberry</t>
-  </si>
-  <si>
-    <t>parachute_jasmine_oil</t>
-  </si>
-  <si>
-    <t>unbranded_kerala_avil</t>
-  </si>
-  <si>
-    <t>lays_chips_cream_and_onion</t>
-  </si>
-  <si>
-    <t>maaza_refresh_mango_drink</t>
-  </si>
-  <si>
-    <t>aquafina_drinking_water_bottle</t>
-  </si>
-  <si>
-    <t>epigamia_milkshake_vanilla</t>
-  </si>
-  <si>
-    <t>150-160 Rs.</t>
-  </si>
-  <si>
-    <t>156-166 Rs.</t>
-  </si>
-  <si>
-    <t>30-40 Rs.</t>
-  </si>
-  <si>
-    <t>130-140 Rs.</t>
-  </si>
-  <si>
-    <t>19-20 Rs.</t>
-  </si>
-  <si>
-    <t>60-70 Rs.</t>
-  </si>
-  <si>
-    <t>oralb_toothbrush_crisscross</t>
+    <t>Sku1_Dettol Soap</t>
+  </si>
+  <si>
+    <t>Sku2_Boost</t>
+  </si>
+  <si>
+    <t>Sku3_Parle-G Biscuits</t>
+  </si>
+  <si>
+    <t>Sku4_Colgate Paste</t>
+  </si>
+  <si>
+    <t>Sku5_Dairy Milk</t>
+  </si>
+  <si>
+    <t>Sku6_Rainbow Tissues</t>
+  </si>
+  <si>
+    <t>Sku7_Ajay tooth Brush</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boost </t>
+  </si>
+  <si>
+    <t>rainbow-tissue</t>
+  </si>
+  <si>
+    <t>dettol-soap</t>
+  </si>
+  <si>
+    <t>parle-G-biscuit</t>
+  </si>
+  <si>
+    <t>colgate-paste</t>
+  </si>
+  <si>
+    <t>dairy-milk-chocolate</t>
+  </si>
+  <si>
+    <t>ajay-tooth-brush</t>
+  </si>
+  <si>
+    <t>dettol</t>
+  </si>
+  <si>
+    <t>boost</t>
+  </si>
+  <si>
+    <t>parle-G</t>
+  </si>
+  <si>
+    <t>Colgate</t>
+  </si>
+  <si>
+    <t>dairy-milk</t>
+  </si>
+  <si>
+    <t>rainbow</t>
+  </si>
+  <si>
+    <t>ajay</t>
+  </si>
+  <si>
+    <t>hygiene-product</t>
+  </si>
+  <si>
+    <t>fnd-product</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -241,6 +166,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -250,7 +182,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -258,25 +190,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFA5A5A5"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -292,18 +243,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB8432CA-EFC4-B645-B18F-F2A137A4F9D5}" name="Table2" displayName="Table2" ref="A1:I10" totalsRowShown="0">
-  <autoFilter ref="A1:I10" xr:uid="{FB8432CA-EFC4-B645-B18F-F2A137A4F9D5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FB8432CA-EFC4-B645-B18F-F2A137A4F9D5}" name="Table2" displayName="Table2" ref="A1:I8" totalsRowShown="0">
+  <autoFilter ref="A1:I8" xr:uid="{FB8432CA-EFC4-B645-B18F-F2A137A4F9D5}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{C7C1EEEA-E750-0E4E-8F6D-9CA97E5A4F41}" name="sku_code"/>
     <tableColumn id="2" xr3:uid="{4F57C4BA-CB09-2C49-AB06-4FA7397EC95E}" name="item_name"/>
     <tableColumn id="3" xr3:uid="{248F82E1-E0AB-AA46-A8FD-BDB281C44F66}" name="brand"/>
     <tableColumn id="4" xr3:uid="{A5AE4ED5-C7D9-FF41-A86D-FB451F0ECA97}" name="sub_category"/>
     <tableColumn id="5" xr3:uid="{E60F1E77-4EF1-5E43-B210-80AE50B82274}" name="category"/>
-    <tableColumn id="6" xr3:uid="{962A032B-8B37-9C4D-A2DD-3CF7F854666C}" name="price_per_unit" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{A0AF6A73-A16E-F049-809F-89912F360B1F}" name="quantity_per_unit" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{39DA38BF-80C0-ED43-86E4-923E1A36836A}" name="upc"/>
-    <tableColumn id="9" xr3:uid="{EE097411-5C0F-5341-A49B-25C7113A3EDF}" name="additional_info"/>
+    <tableColumn id="6" xr3:uid="{962A032B-8B37-9C4D-A2DD-3CF7F854666C}" name="price_per_unit" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{A0AF6A73-A16E-F049-809F-89912F360B1F}" name="quantity_per_unit" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{39DA38BF-80C0-ED43-86E4-923E1A36836A}" name="upc" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{EE097411-5C0F-5341-A49B-25C7113A3EDF}" name="additional_info" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -606,19 +557,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09516FB-AAD9-E048-9A0D-5502BE51B2CF}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="189" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
@@ -642,231 +593,211 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>